<commit_message>
Commenting out stuff not needed yet
</commit_message>
<xml_diff>
--- a/cypress/downloads/NYPDFirmware.xlsx
+++ b/cypress/downloads/NYPDFirmware.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="183">
   <si>
     <t>C Squared Systems - Device Firmware Report</t>
   </si>
@@ -122,6 +122,15 @@
     <t>All Clients &gt;&gt; SH Test &gt;&gt; Eltek Batt Sym</t>
   </si>
   <si>
+    <t>Eltek Sym</t>
+  </si>
+  <si>
+    <t>68.160.220.238:80</t>
+  </si>
+  <si>
+    <t>All Clients &gt;&gt; SH Test &gt;&gt; Eltek Sym</t>
+  </si>
+  <si>
     <t>SH Test</t>
   </si>
   <si>
@@ -317,6 +326,15 @@
     <t>All Clients &gt;&gt; JGF Testing &gt;&gt; Nokia Devices_Writable Properties &gt;&gt; Nokia_SAR-SAS (68.160.220.234)</t>
   </si>
   <si>
+    <t>Nokia_SAR-8_Lab (10.10.190.139)</t>
+  </si>
+  <si>
+    <t>10.10.190.139</t>
+  </si>
+  <si>
+    <t>All Clients &gt;&gt; JGF Testing &gt;&gt; Nokia Devices_Writable Properties &gt;&gt; Nokia_SAR-8_Lab (10.10.190.139)</t>
+  </si>
+  <si>
     <t>Nokia Devices_Writable Properties</t>
   </si>
   <si>
@@ -410,6 +428,9 @@
     <t>All Clients &gt;&gt; 001-KA-Testing &gt;&gt; GDF-1158 &gt;&gt; Ping device 2</t>
   </si>
   <si>
+    <t>All Clients &gt;&gt; 001-KA-Testing &gt;&gt; GDF-1158 &gt;&gt; Nokia_SAR-8 (Q)</t>
+  </si>
+  <si>
     <t>GDF-1158</t>
   </si>
   <si>
@@ -428,10 +449,10 @@
     <t>All Clients &gt;&gt; JC Test &gt;&gt; sub test &gt;&gt; Test1</t>
   </si>
   <si>
-    <t>testing</t>
-  </si>
-  <si>
-    <t>All Clients &gt;&gt; JC Test &gt;&gt; sub test &gt;&gt; testing</t>
+    <t>A loooooooooonnnng name device</t>
+  </si>
+  <si>
+    <t>All Clients &gt;&gt; JC Test &gt;&gt; sub test &gt;&gt; A loooooooooonnnng name device</t>
   </si>
   <si>
     <t>sub test</t>
@@ -928,7 +949,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G92"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -994,7 +1015,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="4">
-        <v>44390.6015625</v>
+        <v>44390.675775463</v>
       </c>
       <c r="G5" t="s">
         <v>13</v>
@@ -1015,7 +1036,7 @@
         <v>17</v>
       </c>
       <c r="F6" s="4">
-        <v>44390.603425926</v>
+        <v>44390.666863426</v>
       </c>
       <c r="G6" t="s">
         <v>18</v>
@@ -1036,7 +1057,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="4">
-        <v>44390.609189815</v>
+        <v>44390.671053241</v>
       </c>
       <c r="G7" t="s">
         <v>20</v>
@@ -1055,7 +1076,7 @@
       </c>
       <c r="E8"/>
       <c r="F8" s="4">
-        <v>44390.600023148</v>
+        <v>44390.664224537</v>
       </c>
       <c r="G8" t="s">
         <v>24</v>
@@ -1076,7 +1097,7 @@
         <v>27</v>
       </c>
       <c r="F9" s="4">
-        <v>44390.612141204</v>
+        <v>44390.675833333</v>
       </c>
       <c r="G9" t="s">
         <v>28</v>
@@ -1097,7 +1118,7 @@
         <v>27</v>
       </c>
       <c r="F10" s="4">
-        <v>44390.608449074</v>
+        <v>44390.672256944</v>
       </c>
       <c r="G10" t="s">
         <v>30</v>
@@ -1118,7 +1139,7 @@
         <v>17</v>
       </c>
       <c r="F11" s="4">
-        <v>44390.61369213</v>
+        <v>44390.676863426</v>
       </c>
       <c r="G11" t="s">
         <v>18</v>
@@ -1139,7 +1160,7 @@
         <v>33</v>
       </c>
       <c r="F12" s="4">
-        <v>44390.605787037</v>
+        <v>44390.672303241</v>
       </c>
       <c r="G12" t="s">
         <v>34</v>
@@ -1151,12 +1172,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
         <v>36</v>
       </c>
-      <c r="D13"/>
-      <c r="E13"/>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
       <c r="F13" s="4">
-        <v>44390.612569444</v>
+        <v>44390.67525463</v>
       </c>
       <c r="G13" t="s">
         <v>37</v>
@@ -1170,50 +1195,48 @@
       <c r="C14" t="s">
         <v>39</v>
       </c>
-      <c r="D14" t="s">
-        <v>40</v>
-      </c>
+      <c r="D14"/>
       <c r="E14"/>
       <c r="F14" s="4">
-        <v>44390.609895833</v>
+        <v>44390.675393519</v>
       </c>
       <c r="G14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15"/>
       <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
         <v>42</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
       </c>
       <c r="E15"/>
       <c r="F15" s="4">
-        <v>44390.610115741</v>
+        <v>44390.673900463</v>
       </c>
       <c r="G15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16"/>
       <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
         <v>46</v>
-      </c>
-      <c r="C16" t="s">
-        <v>43</v>
       </c>
       <c r="D16" t="s">
         <v>47</v>
       </c>
       <c r="E16"/>
       <c r="F16" s="4">
-        <v>44390.606087963</v>
+        <v>44390.669409722</v>
       </c>
       <c r="G16" t="s">
         <v>48</v>
@@ -1225,71 +1248,71 @@
         <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E17"/>
       <c r="F17" s="4">
-        <v>44390.610648148</v>
+        <v>44390.673148148</v>
       </c>
       <c r="G17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18"/>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E18"/>
       <c r="F18" s="4">
-        <v>36526</v>
+        <v>44390.668287037</v>
       </c>
       <c r="G18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19"/>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E19"/>
       <c r="F19" s="4">
-        <v>44390.605277778</v>
+        <v>36526</v>
       </c>
       <c r="G19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20"/>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E20"/>
       <c r="F20" s="4">
-        <v>36526</v>
+        <v>44390.676388889</v>
       </c>
       <c r="G20" t="s">
         <v>57</v>
@@ -1301,26 +1324,26 @@
         <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="E21"/>
       <c r="F21" s="4">
         <v>36526</v>
       </c>
       <c r="G21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22"/>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D22" t="s">
         <v>47</v>
@@ -1330,35 +1353,35 @@
         <v>36526</v>
       </c>
       <c r="G22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23"/>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E23"/>
       <c r="F23" s="4">
         <v>36526</v>
       </c>
       <c r="G23" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24"/>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
         <v>47</v>
@@ -1368,114 +1391,114 @@
         <v>36526</v>
       </c>
       <c r="G24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25"/>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E25"/>
       <c r="F25" s="4">
-        <v>44390.604016204</v>
+        <v>36526</v>
       </c>
       <c r="G25" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26"/>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D26" t="s">
         <v>47</v>
       </c>
       <c r="E26"/>
       <c r="F26" s="4">
-        <v>44390.611527778</v>
+        <v>44390.673032407</v>
       </c>
       <c r="G26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27"/>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D27" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E27"/>
       <c r="F27" s="4">
-        <v>36526</v>
+        <v>44390.667407407</v>
       </c>
       <c r="G27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28"/>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E28"/>
       <c r="F28" s="4">
-        <v>44390.61056713</v>
+        <v>36526</v>
       </c>
       <c r="G28" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29"/>
       <c r="B29" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D29" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E29"/>
       <c r="F29" s="4">
-        <v>36526</v>
+        <v>44390.669814815</v>
       </c>
       <c r="G29" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30"/>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D30" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E30"/>
       <c r="F30" s="4">
@@ -1491,36 +1514,36 @@
         <v>73</v>
       </c>
       <c r="C31" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D31" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E31"/>
       <c r="F31" s="4">
         <v>36526</v>
       </c>
       <c r="G31" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32"/>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C32" t="s">
         <v>22</v>
       </c>
       <c r="D32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E32"/>
       <c r="F32" s="4">
-        <v>44390.605196759</v>
+        <v>36526</v>
       </c>
       <c r="G32" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1529,12 +1552,14 @@
         <v>76</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
-      </c>
-      <c r="D33"/>
+        <v>22</v>
+      </c>
+      <c r="D33" t="s">
+        <v>78</v>
+      </c>
       <c r="E33"/>
       <c r="F33" s="4">
-        <v>44390.613530093</v>
+        <v>44390.668078704</v>
       </c>
       <c r="G33" t="s">
         <v>77</v>
@@ -1543,34 +1568,32 @@
     <row r="34" spans="1:7">
       <c r="A34"/>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D34"/>
       <c r="E34"/>
       <c r="F34" s="4">
-        <v>44390.607268519</v>
+        <v>44390.676388889</v>
       </c>
       <c r="G34" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35"/>
       <c r="B35" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C35" t="s">
         <v>39</v>
       </c>
-      <c r="D35" t="s">
-        <v>81</v>
-      </c>
+      <c r="D35"/>
       <c r="E35"/>
       <c r="F35" s="4">
-        <v>36526</v>
+        <v>44390.670150463</v>
       </c>
       <c r="G35" t="s">
         <v>82</v>
@@ -1579,20 +1602,20 @@
     <row r="36" spans="1:7">
       <c r="A36"/>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D36" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E36"/>
       <c r="F36" s="4">
-        <v>44390.610578704</v>
+        <v>36526</v>
       </c>
       <c r="G36" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1601,31 +1624,31 @@
         <v>83</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
-      </c>
-      <c r="D37"/>
+        <v>42</v>
+      </c>
+      <c r="D37" t="s">
+        <v>84</v>
+      </c>
       <c r="E37"/>
       <c r="F37" s="4">
-        <v>44390.612071759</v>
+        <v>44390.674606481</v>
       </c>
       <c r="G37" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38"/>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C38" t="s">
         <v>39</v>
       </c>
-      <c r="D38" t="s">
-        <v>86</v>
-      </c>
+      <c r="D38"/>
       <c r="E38"/>
       <c r="F38" s="4">
-        <v>44390.502465278</v>
+        <v>44390.674884259</v>
       </c>
       <c r="G38" t="s">
         <v>87</v>
@@ -1637,31 +1660,31 @@
         <v>88</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
-      </c>
-      <c r="D39"/>
+        <v>42</v>
+      </c>
+      <c r="D39" t="s">
+        <v>89</v>
+      </c>
       <c r="E39"/>
       <c r="F39" s="4">
-        <v>44390.604861111</v>
+        <v>44390.502465278</v>
       </c>
       <c r="G39" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40"/>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C40" t="s">
         <v>39</v>
       </c>
-      <c r="D40" t="s">
-        <v>91</v>
-      </c>
+      <c r="D40"/>
       <c r="E40"/>
       <c r="F40" s="4">
-        <v>44390.523912037</v>
+        <v>44390.667685185</v>
       </c>
       <c r="G40" t="s">
         <v>92</v>
@@ -1673,72 +1696,72 @@
         <v>93</v>
       </c>
       <c r="C41" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D41" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="E41"/>
       <c r="F41" s="4">
-        <v>44390.613298611</v>
+        <v>44390.523912037</v>
       </c>
       <c r="G41" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42"/>
       <c r="B42" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C42" t="s">
-        <v>36</v>
-      </c>
-      <c r="D42"/>
+        <v>42</v>
+      </c>
+      <c r="D42" t="s">
+        <v>84</v>
+      </c>
       <c r="E42"/>
       <c r="F42" s="4">
-        <v>44390.606886574</v>
+        <v>44390.677314815</v>
       </c>
       <c r="G42" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43"/>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="C43" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" t="s">
-        <v>44</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D43"/>
       <c r="E43"/>
       <c r="F43" s="4">
-        <v>44390.612349537</v>
+        <v>44390.669710648</v>
       </c>
       <c r="G43" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44"/>
       <c r="B44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" t="s">
         <v>46</v>
-      </c>
-      <c r="C44" t="s">
-        <v>43</v>
       </c>
       <c r="D44" t="s">
         <v>47</v>
       </c>
       <c r="E44"/>
       <c r="F44" s="4">
-        <v>44390.609328704</v>
+        <v>44390.671493056</v>
       </c>
       <c r="G44" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1747,88 +1770,86 @@
         <v>49</v>
       </c>
       <c r="C45" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D45" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E45"/>
       <c r="F45" s="4">
-        <v>44390.612152778</v>
+        <v>44390.676550926</v>
       </c>
       <c r="G45" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46"/>
       <c r="B46" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="C46" t="s">
-        <v>36</v>
-      </c>
-      <c r="D46"/>
+        <v>46</v>
+      </c>
+      <c r="D46" t="s">
+        <v>47</v>
+      </c>
       <c r="E46"/>
       <c r="F46" s="4">
-        <v>44390.610300926</v>
+        <v>44390.669803241</v>
       </c>
       <c r="G46" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47"/>
       <c r="B47" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C47" t="s">
-        <v>36</v>
-      </c>
-      <c r="D47"/>
+        <v>46</v>
+      </c>
+      <c r="D47" t="s">
+        <v>104</v>
+      </c>
       <c r="E47"/>
       <c r="F47" s="4">
-        <v>44390.61119213</v>
+        <v>44390.672835648</v>
       </c>
       <c r="G47" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48"/>
       <c r="B48" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C48" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" t="s">
-        <v>105</v>
-      </c>
-      <c r="E48" t="s">
-        <v>27</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D48"/>
+      <c r="E48"/>
       <c r="F48" s="4">
-        <v>44390.613414352</v>
+        <v>44390.67318287</v>
       </c>
       <c r="G48" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49"/>
       <c r="B49" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C49" t="s">
-        <v>22</v>
-      </c>
-      <c r="D49" t="s">
-        <v>108</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D49"/>
       <c r="E49"/>
       <c r="F49" s="4">
-        <v>36526</v>
+        <v>44390.6740625</v>
       </c>
       <c r="G49" t="s">
         <v>109</v>
@@ -1837,489 +1858,493 @@
     <row r="50" spans="1:7">
       <c r="A50"/>
       <c r="B50" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C50" t="s">
         <v>22</v>
       </c>
       <c r="D50" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E50" t="s">
         <v>27</v>
       </c>
       <c r="F50" s="4">
-        <v>44390.613414352</v>
+        <v>44390.669236111</v>
       </c>
       <c r="G50" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51"/>
       <c r="B51" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C51" t="s">
         <v>22</v>
       </c>
       <c r="D51" t="s">
-        <v>105</v>
-      </c>
-      <c r="E51" t="s">
-        <v>27</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="E51"/>
       <c r="F51" s="4">
-        <v>44390.613414352</v>
+        <v>36526</v>
       </c>
       <c r="G51" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52"/>
       <c r="B52" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C52" t="s">
         <v>22</v>
       </c>
       <c r="D52" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E52" t="s">
         <v>27</v>
       </c>
       <c r="F52" s="4">
-        <v>44390.606446759</v>
+        <v>44390.669328704</v>
       </c>
       <c r="G52" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53"/>
       <c r="B53" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="C53" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D53" t="s">
-        <v>44</v>
-      </c>
-      <c r="E53"/>
+        <v>111</v>
+      </c>
+      <c r="E53" t="s">
+        <v>27</v>
+      </c>
       <c r="F53" s="4">
-        <v>44390.606041667</v>
+        <v>44390.669236111</v>
       </c>
       <c r="G53" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54"/>
       <c r="B54" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
       <c r="C54" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D54" t="s">
-        <v>47</v>
-      </c>
-      <c r="E54"/>
+        <v>111</v>
+      </c>
+      <c r="E54" t="s">
+        <v>27</v>
+      </c>
       <c r="F54" s="4">
-        <v>44390.607986111</v>
+        <v>44390.673900463</v>
       </c>
       <c r="G54" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55"/>
       <c r="B55" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C55" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D55" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E55"/>
       <c r="F55" s="4">
-        <v>44390.606354167</v>
+        <v>44390.675671296</v>
       </c>
       <c r="G55" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56"/>
       <c r="B56" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C56" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="D56" t="s">
-        <v>117</v>
+        <v>50</v>
       </c>
       <c r="E56"/>
       <c r="F56" s="4">
-        <v>44390.609108796</v>
+        <v>44390.675231481</v>
       </c>
       <c r="G56" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57"/>
       <c r="B57" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="C57" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D57" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E57"/>
       <c r="F57" s="4">
-        <v>44390.608657407</v>
+        <v>44390.677199074</v>
       </c>
       <c r="G57" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58"/>
       <c r="B58" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C58" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D58" t="s">
-        <v>44</v>
+        <v>123</v>
       </c>
       <c r="E58"/>
       <c r="F58" s="4">
-        <v>36526</v>
+        <v>44390.673310185</v>
       </c>
       <c r="G58" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59"/>
       <c r="B59" t="s">
-        <v>62</v>
+        <v>124</v>
       </c>
       <c r="C59" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D59" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E59"/>
       <c r="F59" s="4">
-        <v>44390.613877315</v>
+        <v>44390.668159722</v>
       </c>
       <c r="G59" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60"/>
       <c r="B60" t="s">
-        <v>121</v>
+        <v>65</v>
       </c>
       <c r="C60" t="s">
-        <v>36</v>
-      </c>
-      <c r="D60"/>
+        <v>46</v>
+      </c>
+      <c r="D60" t="s">
+        <v>47</v>
+      </c>
       <c r="E60"/>
       <c r="F60" s="4">
-        <v>44390.613530093</v>
+        <v>36526</v>
       </c>
       <c r="G60" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61"/>
       <c r="B61" t="s">
-        <v>123</v>
+        <v>65</v>
       </c>
       <c r="C61" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="D61" t="s">
-        <v>108</v>
+        <v>47</v>
       </c>
       <c r="E61"/>
       <c r="F61" s="4">
-        <v>36526</v>
+        <v>44390.671331019</v>
       </c>
       <c r="G61" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62"/>
       <c r="B62" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C62" t="s">
-        <v>22</v>
-      </c>
-      <c r="D62" t="s">
-        <v>105</v>
-      </c>
-      <c r="E62" t="s">
-        <v>27</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D62"/>
+      <c r="E62"/>
       <c r="F62" s="4">
-        <v>44390.605856481</v>
+        <v>44390.676388889</v>
       </c>
       <c r="G62" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63"/>
       <c r="B63" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
       <c r="C63" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D63" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="E63"/>
       <c r="F63" s="4">
         <v>36526</v>
       </c>
       <c r="G63" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64"/>
       <c r="B64" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C64" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="D64" t="s">
-        <v>127</v>
-      </c>
-      <c r="E64"/>
+        <v>111</v>
+      </c>
+      <c r="E64" t="s">
+        <v>27</v>
+      </c>
       <c r="F64" s="4">
-        <v>36526</v>
+        <v>44390.673194444</v>
       </c>
       <c r="G64" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65"/>
       <c r="B65" t="s">
-        <v>126</v>
+        <v>67</v>
       </c>
       <c r="C65" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D65" t="s">
-        <v>127</v>
+        <v>50</v>
       </c>
       <c r="E65"/>
       <c r="F65" s="4">
-        <v>44390.612476852</v>
+        <v>36526</v>
       </c>
       <c r="G65" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66"/>
       <c r="B66" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C66" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D66" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E66"/>
       <c r="F66" s="4">
-        <v>44390.607106481</v>
+        <v>36526</v>
       </c>
       <c r="G66" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67"/>
       <c r="B67" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C67" t="s">
-        <v>36</v>
-      </c>
-      <c r="D67"/>
+        <v>42</v>
+      </c>
+      <c r="D67" t="s">
+        <v>133</v>
+      </c>
       <c r="E67"/>
       <c r="F67" s="4">
-        <v>44390.61068287</v>
+        <v>44390.676493056</v>
       </c>
       <c r="G67" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68"/>
       <c r="B68" t="s">
+        <v>135</v>
+      </c>
+      <c r="C68" t="s">
+        <v>42</v>
+      </c>
+      <c r="D68" t="s">
         <v>133</v>
       </c>
-      <c r="C68" t="s">
-        <v>36</v>
-      </c>
-      <c r="D68"/>
       <c r="E68"/>
       <c r="F68" s="4">
-        <v>44390.612569444</v>
+        <v>44390.671134259</v>
       </c>
       <c r="G68" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69"/>
       <c r="B69" t="s">
-        <v>135</v>
+        <v>69</v>
       </c>
       <c r="C69" t="s">
-        <v>36</v>
-      </c>
-      <c r="D69"/>
+        <v>46</v>
+      </c>
+      <c r="D69" t="s">
+        <v>47</v>
+      </c>
       <c r="E69"/>
       <c r="F69" s="4">
-        <v>44390.612071759</v>
+        <v>44390.667893519</v>
       </c>
       <c r="G69" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70"/>
       <c r="B70" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C70" t="s">
         <v>39</v>
       </c>
-      <c r="D70" t="s">
-        <v>127</v>
-      </c>
+      <c r="D70"/>
       <c r="E70"/>
       <c r="F70" s="4">
-        <v>44390.612476852</v>
+        <v>44390.673553241</v>
       </c>
       <c r="G70" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71"/>
       <c r="B71" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C71" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D71"/>
       <c r="E71"/>
       <c r="F71" s="4">
-        <v>44390.612071759</v>
+        <v>44390.675393519</v>
       </c>
       <c r="G71" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72"/>
       <c r="B72" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C72" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D72"/>
       <c r="E72"/>
       <c r="F72" s="4">
-        <v>44390.612071759</v>
+        <v>44390.674884259</v>
       </c>
       <c r="G72" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73"/>
       <c r="B73" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C73" t="s">
-        <v>36</v>
-      </c>
-      <c r="D73"/>
+        <v>42</v>
+      </c>
+      <c r="D73" t="s">
+        <v>133</v>
+      </c>
       <c r="E73"/>
       <c r="F73" s="4">
-        <v>44390.612071759</v>
+        <v>44390.670196759</v>
       </c>
       <c r="G73" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74"/>
       <c r="B74" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C74" t="s">
         <v>39</v>
       </c>
-      <c r="D74" t="s">
-        <v>127</v>
-      </c>
+      <c r="D74"/>
       <c r="E74"/>
       <c r="F74" s="4">
-        <v>44390.612916667</v>
+        <v>44390.674884259</v>
       </c>
       <c r="G74" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75"/>
       <c r="B75" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C75" t="s">
         <v>39</v>
       </c>
-      <c r="D75" t="s">
-        <v>71</v>
-      </c>
+      <c r="D75"/>
       <c r="E75"/>
       <c r="F75" s="4">
-        <v>44389.618252315</v>
+        <v>44390.674884259</v>
       </c>
       <c r="G75" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2330,301 +2355,356 @@
       <c r="C76" t="s">
         <v>39</v>
       </c>
-      <c r="D76" t="s">
-        <v>127</v>
-      </c>
+      <c r="D76"/>
       <c r="E76"/>
       <c r="F76" s="4">
-        <v>44390.61474537</v>
+        <v>44390.674884259</v>
       </c>
       <c r="G76" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77"/>
       <c r="B77" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C77" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D77" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E77"/>
       <c r="F77" s="4">
-        <v>44390.612476852</v>
+        <v>44390.674606481</v>
       </c>
       <c r="G77" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78"/>
       <c r="B78" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C78" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D78" t="s">
-        <v>127</v>
+        <v>74</v>
       </c>
       <c r="E78"/>
       <c r="F78" s="4">
-        <v>44390.607939815</v>
+        <v>44389.618252315</v>
       </c>
       <c r="G78" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79"/>
       <c r="B79" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C79" t="s">
-        <v>36</v>
-      </c>
-      <c r="D79"/>
+        <v>42</v>
+      </c>
+      <c r="D79" t="s">
+        <v>133</v>
+      </c>
       <c r="E79"/>
       <c r="F79" s="4">
-        <v>44390.612569444</v>
+        <v>44390.674027778</v>
       </c>
       <c r="G79" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80"/>
       <c r="B80" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C80" t="s">
-        <v>36</v>
-      </c>
-      <c r="D80"/>
+        <v>42</v>
+      </c>
+      <c r="D80" t="s">
+        <v>133</v>
+      </c>
       <c r="E80"/>
       <c r="F80" s="4">
-        <v>44390.612569444</v>
+        <v>44390.674155093</v>
       </c>
       <c r="G80" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81"/>
       <c r="B81" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
       <c r="C81" t="s">
-        <v>36</v>
-      </c>
-      <c r="D81"/>
+        <v>42</v>
+      </c>
+      <c r="D81" t="s">
+        <v>133</v>
+      </c>
       <c r="E81"/>
       <c r="F81" s="4">
-        <v>44390.612071759</v>
+        <v>44390.674097222</v>
       </c>
       <c r="G81" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82"/>
       <c r="B82" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C82" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D82"/>
       <c r="E82"/>
       <c r="F82" s="4">
-        <v>44390.61119213</v>
+        <v>44390.675381944</v>
       </c>
       <c r="G82" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83"/>
       <c r="B83" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C83" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D83"/>
       <c r="E83"/>
       <c r="F83" s="4">
-        <v>44390.610613426</v>
+        <v>44390.675393519</v>
       </c>
       <c r="G83" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84"/>
       <c r="B84" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C84" t="s">
         <v>39</v>
       </c>
-      <c r="D84" t="s">
-        <v>127</v>
-      </c>
+      <c r="D84"/>
       <c r="E84"/>
       <c r="F84" s="4">
-        <v>44390.611145833</v>
+        <v>44390.674884259</v>
       </c>
       <c r="G84" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85"/>
       <c r="B85" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="C85" t="s">
         <v>39</v>
       </c>
-      <c r="D85" t="s">
-        <v>127</v>
-      </c>
+      <c r="D85"/>
       <c r="E85"/>
       <c r="F85" s="4">
-        <v>44390.611145833</v>
+        <v>44390.6740625</v>
       </c>
       <c r="G85" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86"/>
       <c r="B86" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="C86" t="s">
         <v>39</v>
       </c>
-      <c r="D86" t="s">
-        <v>127</v>
-      </c>
+      <c r="D86"/>
       <c r="E86"/>
       <c r="F86" s="4">
-        <v>44390.611145833</v>
+        <v>44390.67349537</v>
       </c>
       <c r="G86" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87"/>
       <c r="B87" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C87" t="s">
-        <v>36</v>
-      </c>
-      <c r="D87"/>
+        <v>42</v>
+      </c>
+      <c r="D87" t="s">
+        <v>133</v>
+      </c>
       <c r="E87"/>
       <c r="F87" s="4">
-        <v>44390.612569444</v>
+        <v>44390.674664352</v>
       </c>
       <c r="G87" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88"/>
       <c r="B88" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="C88" t="s">
-        <v>36</v>
-      </c>
-      <c r="D88"/>
+        <v>42</v>
+      </c>
+      <c r="D88" t="s">
+        <v>133</v>
+      </c>
       <c r="E88"/>
       <c r="F88" s="4">
-        <v>44390.612384259</v>
+        <v>44390.674664352</v>
       </c>
       <c r="G88" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89"/>
       <c r="B89" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="C89" t="s">
-        <v>36</v>
-      </c>
-      <c r="D89"/>
+        <v>42</v>
+      </c>
+      <c r="D89" t="s">
+        <v>133</v>
+      </c>
       <c r="E89"/>
       <c r="F89" s="4">
-        <v>44390.612384259</v>
+        <v>44390.675173611</v>
       </c>
       <c r="G89" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90"/>
       <c r="B90" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C90" t="s">
-        <v>15</v>
-      </c>
-      <c r="D90" t="s">
-        <v>16</v>
-      </c>
-      <c r="E90" t="s">
-        <v>17</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D90"/>
+      <c r="E90"/>
       <c r="F90" s="4">
-        <v>44390.541516204</v>
+        <v>44390.675393519</v>
       </c>
       <c r="G90" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91"/>
       <c r="B91" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C91" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D91"/>
       <c r="E91"/>
       <c r="F91" s="4">
-        <v>44390.614583333</v>
+        <v>44390.675266204</v>
       </c>
       <c r="G91" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92"/>
       <c r="B92" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C92" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D92"/>
       <c r="E92"/>
       <c r="F92" s="4">
-        <v>44390.612569444</v>
+        <v>44390.675266204</v>
       </c>
       <c r="G92" t="s">
-        <v>175</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93"/>
+      <c r="B93" t="s">
+        <v>178</v>
+      </c>
+      <c r="C93" t="s">
+        <v>15</v>
+      </c>
+      <c r="D93" t="s">
+        <v>16</v>
+      </c>
+      <c r="E93" t="s">
+        <v>17</v>
+      </c>
+      <c r="F93" s="4">
+        <v>44390.541516204</v>
+      </c>
+      <c r="G93" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94"/>
+      <c r="B94" t="s">
+        <v>180</v>
+      </c>
+      <c r="C94" t="s">
+        <v>39</v>
+      </c>
+      <c r="D94"/>
+      <c r="E94"/>
+      <c r="F94" s="4">
+        <v>44390.677465278</v>
+      </c>
+      <c r="G94" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95"/>
+      <c r="B95" t="s">
+        <v>182</v>
+      </c>
+      <c r="C95" t="s">
+        <v>39</v>
+      </c>
+      <c r="D95"/>
+      <c r="E95"/>
+      <c r="F95" s="4">
+        <v>44390.675393519</v>
+      </c>
+      <c r="G95" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>